<commit_message>
Recoded the bitmap such that the condition is fully identified with the bitcode, i.e., one is able to tell the full condition from the MEG stream. The bitcode is now taken from cond-file. Note that this requires a configuration of the MEG machine.
</commit_message>
<xml_diff>
--- a/cond-files/cond_meg1.xlsx
+++ b/cond-files/cond_meg1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gd\Projects\pm\pm\cond-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7132E07-05FA-484F-B214-530965F9DBAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B55B702-2F29-4F8C-B829-6C0E226DF4CF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13850" yWindow="16010" windowWidth="8117" windowHeight="10669" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cond_pm1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="6">
   <si>
     <t>L</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>stim_c</t>
+  </si>
+  <si>
+    <t>bitcode</t>
   </si>
 </sst>
 </file>
@@ -907,15 +910,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A33"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -925,8 +928,11 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -936,8 +942,11 @@
       <c r="C2">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -947,8 +956,11 @@
       <c r="C3">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -958,8 +970,11 @@
       <c r="C4">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -969,8 +984,11 @@
       <c r="C5">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -980,8 +998,11 @@
       <c r="C6">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -991,8 +1012,11 @@
       <c r="C7">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1002,8 +1026,11 @@
       <c r="C8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1013,8 +1040,11 @@
       <c r="C9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1024,8 +1054,11 @@
       <c r="C10">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1035,8 +1068,11 @@
       <c r="C11">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1046,8 +1082,11 @@
       <c r="C12">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1057,8 +1096,11 @@
       <c r="C13">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1068,8 +1110,11 @@
       <c r="C14">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1079,8 +1124,11 @@
       <c r="C15">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1090,8 +1138,11 @@
       <c r="C16">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1101,8 +1152,11 @@
       <c r="C17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1112,8 +1166,11 @@
       <c r="C18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1123,8 +1180,11 @@
       <c r="C19">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1134,8 +1194,11 @@
       <c r="C20">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1145,8 +1208,11 @@
       <c r="C21">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1156,8 +1222,11 @@
       <c r="C22">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1167,8 +1236,11 @@
       <c r="C23">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1178,8 +1250,11 @@
       <c r="C24">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1189,8 +1264,11 @@
       <c r="C25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1200,8 +1278,11 @@
       <c r="C26">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1211,8 +1292,11 @@
       <c r="C27">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1222,8 +1306,11 @@
       <c r="C28">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1233,8 +1320,11 @@
       <c r="C29">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1244,8 +1334,11 @@
       <c r="C30">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1255,8 +1348,11 @@
       <c r="C31">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1266,8 +1362,11 @@
       <c r="C32">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1276,6 +1375,9 @@
       </c>
       <c r="C33">
         <v>100</v>
+      </c>
+      <c r="D33">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>